<commit_message>
Mejoras en búsqueda de CI
</commit_message>
<xml_diff>
--- a/results/contadores.xlsx
+++ b/results/contadores.xlsx
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
         <v>4</v>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios y arreglos varios
- Cambios en búsqueda para que encuentre solamente positivos.
- Arreglos en conteo.
- Configuración en fichero YML.
- Etc.
</commit_message>
<xml_diff>
--- a/results/contadores.xlsx
+++ b/results/contadores.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>38</v>
+        <v>176</v>
       </c>
       <c r="C15" t="n">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ arreglos en 'parseo' de ficheros YML de CI
</commit_message>
<xml_diff>
--- a/results/contadores.xlsx
+++ b/results/contadores.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>221</v>
+        <v>130</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>279</v>
+        <v>153</v>
       </c>
       <c r="C15" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
YML parser + API rate
Arreglos en el YML parser y en la gestión del API rate de GitHub.
</commit_message>
<xml_diff>
--- a/results/contadores.xlsx
+++ b/results/contadores.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>153</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>